<commit_message>
character archetypes and plots
</commit_message>
<xml_diff>
--- a/data/gender_topics25_processed.xlsx
+++ b/data/gender_topics25_processed.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weizhensheng/Documents/20sp/DATS599/Film-Screenplay-Analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{53C17EE1-811D-8E48-9960-2D9BDD4BDFE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D821FE-DF59-B046-A7EE-5D898C688FE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27480" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gender_topics25" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">gender_topics25!$A$1:$H$26</definedName>
+  </definedNames>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
   <si>
     <t>top_topic</t>
   </si>
@@ -110,12 +113,78 @@
   </si>
   <si>
     <t>diff (% of female %)</t>
+  </si>
+  <si>
+    <t>mapped common</t>
+  </si>
+  <si>
+    <t>mapped hero</t>
+  </si>
+  <si>
+    <t>mapped heroine</t>
+  </si>
+  <si>
+    <t>orphan</t>
+  </si>
+  <si>
+    <t>jester</t>
+  </si>
+  <si>
+    <t>ruler</t>
+  </si>
+  <si>
+    <t>rebel</t>
+  </si>
+  <si>
+    <t>dionysus</t>
+  </si>
+  <si>
+    <t>hera</t>
+  </si>
+  <si>
+    <t>hephestus</t>
+  </si>
+  <si>
+    <t>demeter</t>
+  </si>
+  <si>
+    <t>hermes</t>
+  </si>
+  <si>
+    <t>ares</t>
+  </si>
+  <si>
+    <t>zeus</t>
+  </si>
+  <si>
+    <t>athena</t>
+  </si>
+  <si>
+    <t>apollo</t>
+  </si>
+  <si>
+    <t>persephone</t>
+  </si>
+  <si>
+    <t>everyperson</t>
+  </si>
+  <si>
+    <t>poseidon</t>
+  </si>
+  <si>
+    <t>artemis</t>
+  </si>
+  <si>
+    <t>hero</t>
+  </si>
+  <si>
+    <t>innocent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -252,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +504,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,11 +680,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -958,21 +1042,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="121.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="115.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -988,170 +1075,254 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1.85614849187935</v>
+      </c>
+      <c r="C2">
+        <v>0.80508474576271105</v>
+      </c>
+      <c r="D2">
+        <f>(B2-C2)*100/B2</f>
+        <v>56.626059322033932</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>17.865429234338698</v>
+      </c>
+      <c r="C3">
+        <v>11.4406779661016</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D26" si="0">(B3-C3)*100/B3</f>
+        <v>35.961919436496068</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="6">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.17401392111368899</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.12711864406779599</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" si="0"/>
+        <v>26.949152542373191</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0.522041763341067</v>
+      </c>
+      <c r="C5">
+        <v>0.38135593220338898</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>26.949152542373007</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>0.29002320185614799</v>
       </c>
-      <c r="C2">
+      <c r="C6">
         <v>0.25423728813559299</v>
       </c>
-      <c r="D2">
-        <f>(B2-C2)/B2</f>
-        <v>0.12338983050847388</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>12.338983050847387</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1.10208816705336</v>
-      </c>
-      <c r="C3">
-        <v>1.2711864406779601</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D26" si="0">(B3-C3)/B3</f>
-        <v>-0.15343443354147981</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>4.4663573085846799</v>
-      </c>
-      <c r="C4">
-        <v>5.42372881355932</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>-0.21435174994497169</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>19.199535962877</v>
+      </c>
+      <c r="C7">
+        <v>17.161016949152501</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>10.617543140969918</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0.17401392111368899</v>
-      </c>
-      <c r="C5">
-        <v>0.21186440677966101</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>-0.217514124293786</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>16.0092807424593</v>
+      </c>
+      <c r="C8">
+        <v>16.059322033898301</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-0.31257676246680621</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>0.87006960556844504</v>
+      </c>
+      <c r="C9">
+        <v>0.88983050847457601</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-2.2711864406779876</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1.85614849187935</v>
-      </c>
-      <c r="C6">
-        <v>0.80508474576271105</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0.56626059322033939</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>25.522041763341001</v>
-      </c>
-      <c r="C7">
-        <v>28.093220338982999</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>-0.10074345146379127</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0.17401392111368899</v>
-      </c>
-      <c r="C8">
-        <v>0.25423728813559299</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>-0.46101694915254193</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>19.199535962877</v>
-      </c>
-      <c r="C9">
-        <v>17.161016949152501</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.10617543140969918</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>9</v>
-      </c>
       <c r="B10">
-        <v>17.865429234338698</v>
+        <v>0.63805104408352598</v>
       </c>
       <c r="C10">
-        <v>11.4406779661016</v>
+        <v>0.677966101694915</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.35961919436496065</v>
+        <v>-6.2557781201849778</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1163,283 +1334,420 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>-8.7268427276313204E-2</v>
-      </c>
-      <c r="E11" t="s">
+        <v>-8.7268427276313201</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>0.81206496519721505</v>
+        <v>25.522041763341001</v>
       </c>
       <c r="C12">
-        <v>1.1016949152542299</v>
+        <v>28.093220338982999</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>-0.3566585956416386</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>-10.074345146379127</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>1.10208816705336</v>
+      </c>
+      <c r="C13">
+        <v>1.2711864406779601</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-15.343443354147981</v>
+      </c>
+      <c r="E13" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>0.522041763341067</v>
-      </c>
-      <c r="C13">
-        <v>1.3983050847457601</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>-1.6785310734463241</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>4.4663573085846799</v>
+      </c>
+      <c r="C14">
+        <v>5.42372881355932</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-21.435174994497167</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="6">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.17401392111368899</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.21186440677966101</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="0"/>
+        <v>-21.7514124293786</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>0.63805104408352598</v>
-      </c>
-      <c r="C14">
-        <v>0.677966101694915</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>-6.255778120184978E-2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0.17401392111368899</v>
-      </c>
-      <c r="C15">
-        <v>0.12711864406779599</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0.26949152542373189</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16">
-        <v>0.522041763341067</v>
+        <v>2.8422273781902501</v>
       </c>
       <c r="C16">
-        <v>0.38135593220338898</v>
+        <v>3.5593220338983</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0.26949152542373006</v>
+        <v>-25.230024213075108</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>16</v>
-      </c>
       <c r="B17">
-        <v>0.23201856148491801</v>
+        <v>0.92807424593967502</v>
       </c>
       <c r="C17">
-        <v>0.50847457627118597</v>
+        <v>1.1864406779661001</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>-1.1915254237288191</v>
+        <v>-27.838983050847304</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>0.46403712296983701</v>
       </c>
       <c r="C18">
+        <v>0.59322033898305004</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-27.838983050847443</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>0.81206496519721505</v>
+      </c>
+      <c r="C19">
+        <v>1.1016949152542299</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-35.66585956416386</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="6">
+        <v>7</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.17401392111368899</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.25423728813559299</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" si="0"/>
+        <v>-46.101694915254186</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>0.58004640371229699</v>
+      </c>
+      <c r="C21">
+        <v>0.84745762711864403</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-46.101694915254228</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>1.27610208816705</v>
+      </c>
+      <c r="C22">
+        <v>2.2457627118643999</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-75.986132511556178</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="4">
+        <v>16</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.23201856148491801</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.50847457627118597</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>-119.1525423728819</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>0.522041763341067</v>
+      </c>
+      <c r="C24">
+        <v>1.1864406779661001</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-127.26930320150642</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>0.522041763341067</v>
+      </c>
+      <c r="C25">
+        <v>1.3983050847457601</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>-167.85310734463243</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>0.46403712296983701</v>
+      </c>
+      <c r="C26">
         <v>1.6101694915254201</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>-2.4699152542372844</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-246.99152542372846</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>0.87006960556844504</v>
-      </c>
-      <c r="C19">
-        <v>0.88983050847457601</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>-2.2711864406779875E-2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>0.92807424593967502</v>
-      </c>
-      <c r="C20">
-        <v>1.1864406779661001</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>-0.27838983050847305</v>
-      </c>
-      <c r="E20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>0.522041763341067</v>
-      </c>
-      <c r="C21">
-        <v>1.1864406779661001</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>-1.272693032015064</v>
-      </c>
-      <c r="E21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>0.58004640371229699</v>
-      </c>
-      <c r="C22">
-        <v>0.84745762711864403</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>-0.46101694915254232</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>2.8422273781902501</v>
-      </c>
-      <c r="C23">
-        <v>3.5593220338983</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>-0.25230024213075108</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>1.27610208816705</v>
-      </c>
-      <c r="C24">
-        <v>2.2457627118643999</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>-0.7598613251155617</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>0.46403712296983701</v>
-      </c>
-      <c r="C25">
-        <v>0.59322033898305004</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>-0.27838983050847443</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>16.0092807424593</v>
-      </c>
-      <c r="C26">
-        <v>16.059322033898301</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>-3.1257676246680623E-3</v>
-      </c>
-      <c r="E26" t="s">
-        <v>6</v>
+      <c r="F26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H26" xr:uid="{829A0EC0-404C-F24F-9793-579A6F3CB28D}">
+    <sortState ref="A2:H26">
+      <sortCondition descending="1" ref="D1:D26"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="B2:B26">
     <cfRule type="colorScale" priority="2">
       <colorScale>

</xml_diff>